<commit_message>
Changed the data #FirstEver #ThisAgain
</commit_message>
<xml_diff>
--- a/EditedData.xlsx
+++ b/EditedData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Desktop\CFG2K17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\team-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicator Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="27">
   <si>
     <t/>
   </si>
@@ -87,103 +87,16 @@
     <t>Colombia</t>
   </si>
   <si>
-    <t>2015 DHS</t>
-  </si>
-  <si>
-    <t>2010 DHS</t>
-  </si>
-  <si>
-    <t>2005 DHS</t>
-  </si>
-  <si>
-    <t>2000 DHS</t>
-  </si>
-  <si>
-    <t>1995 DHS</t>
-  </si>
-  <si>
-    <t>1990 DHS</t>
-  </si>
-  <si>
-    <t>1986 DHS</t>
-  </si>
-  <si>
     <t>India</t>
-  </si>
-  <si>
-    <t>2005-06 DHS</t>
-  </si>
-  <si>
-    <t>1998-99 DHS</t>
-  </si>
-  <si>
-    <t>1992-93 DHS</t>
   </si>
   <si>
     <t>Indonesia</t>
   </si>
   <si>
-    <t>2012 DHS</t>
-  </si>
-  <si>
-    <t>2007 DHS</t>
-  </si>
-  <si>
-    <t>2002-03 DHS</t>
-  </si>
-  <si>
-    <t>1997 DHS</t>
-  </si>
-  <si>
-    <t>1994 DHS</t>
-  </si>
-  <si>
-    <t>1991 DHS</t>
-  </si>
-  <si>
-    <t>1987 DHS</t>
-  </si>
-  <si>
     <t>Kenya</t>
   </si>
   <si>
-    <t>2015 MIS</t>
-  </si>
-  <si>
-    <t>2014 DHS</t>
-  </si>
-  <si>
-    <t>2008-09 DHS</t>
-  </si>
-  <si>
-    <t>2003 DHS</t>
-  </si>
-  <si>
-    <t>1998 DHS</t>
-  </si>
-  <si>
-    <t>1993 DHS</t>
-  </si>
-  <si>
-    <t>1989 DHS</t>
-  </si>
-  <si>
     <t>Senegal</t>
-  </si>
-  <si>
-    <t>2016 DHS</t>
-  </si>
-  <si>
-    <t>2012-13 DHS</t>
-  </si>
-  <si>
-    <t>2010-11 DHS</t>
-  </si>
-  <si>
-    <t>2008-09 MIS</t>
-  </si>
-  <si>
-    <t>2006 MIS</t>
   </si>
   <si>
     <t>Indicator</t>
@@ -192,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -579,14 +492,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AF15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AH39" sqref="AH39"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -596,7 +509,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -782,8 +695,8 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
+      <c r="B3" s="1">
+        <v>2015</v>
       </c>
       <c r="C3" s="2">
         <v>81</v>
@@ -887,8 +800,8 @@
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
+      <c r="B4" s="1">
+        <v>2010</v>
       </c>
       <c r="C4" s="2">
         <v>79.099999999999994</v>
@@ -992,8 +905,8 @@
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
+      <c r="B5" s="1">
+        <v>2005</v>
       </c>
       <c r="C5" s="2">
         <v>78.2</v>
@@ -1097,8 +1010,8 @@
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
+      <c r="B6" s="1">
+        <v>2000</v>
       </c>
       <c r="C6" s="2">
         <v>76.900000000000006</v>
@@ -1202,8 +1115,8 @@
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
+      <c r="B7" s="1">
+        <v>1995</v>
       </c>
       <c r="C7" s="2">
         <v>72.2</v>
@@ -1307,8 +1220,8 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+      <c r="B8" s="1">
+        <v>1990</v>
       </c>
       <c r="C8" s="2">
         <v>66.099999999999994</v>
@@ -1412,8 +1325,8 @@
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
+      <c r="B9" s="1">
+        <v>1986</v>
       </c>
       <c r="C9" s="2">
         <v>64.8</v>
@@ -1517,10 +1430,10 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2006</v>
       </c>
       <c r="C10" s="2">
         <v>56.3</v>
@@ -1624,10 +1537,10 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1999</v>
       </c>
       <c r="C11" s="2">
         <v>48.2</v>
@@ -1729,10 +1642,10 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1993</v>
       </c>
       <c r="C12" s="2">
         <v>40.700000000000003</v>
@@ -1834,10 +1747,10 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2012</v>
       </c>
       <c r="C13" s="2">
         <v>61.9</v>
@@ -1941,10 +1854,10 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2007</v>
       </c>
       <c r="C14" s="2">
         <v>61.4</v>
@@ -2048,10 +1961,10 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2003</v>
       </c>
       <c r="C15" s="2">
         <v>60.3</v>
@@ -2155,10 +2068,10 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1997</v>
       </c>
       <c r="C16" s="2">
         <v>57.4</v>
@@ -2260,10 +2173,10 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1994</v>
       </c>
       <c r="C17" s="2">
         <v>54.7</v>
@@ -2365,10 +2278,10 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1991</v>
       </c>
       <c r="C18" s="2">
         <v>49.7</v>
@@ -2470,10 +2383,10 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1987</v>
       </c>
       <c r="C19" s="2">
         <v>47.7</v>
@@ -2577,10 +2490,10 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2015</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>0</v>
@@ -2684,10 +2597,10 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2014</v>
       </c>
       <c r="C21" s="2">
         <v>58</v>
@@ -2791,10 +2704,10 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2009</v>
       </c>
       <c r="C22" s="2">
         <v>45.5</v>
@@ -2898,10 +2811,10 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2003</v>
       </c>
       <c r="C23" s="2">
         <v>39.299999999999997</v>
@@ -3005,10 +2918,10 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1998</v>
       </c>
       <c r="C24" s="2">
         <v>39</v>
@@ -3110,10 +3023,10 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1993</v>
       </c>
       <c r="C25" s="2">
         <v>32.700000000000003</v>
@@ -3215,10 +3128,10 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1989</v>
       </c>
       <c r="C26" s="2">
         <v>26.9</v>
@@ -3322,10 +3235,10 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2016</v>
       </c>
       <c r="C27" s="2">
         <v>25.1</v>
@@ -3429,10 +3342,10 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2015</v>
       </c>
       <c r="C28" s="2">
         <v>23.3</v>
@@ -3536,10 +3449,10 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2014</v>
       </c>
       <c r="C29" s="2">
         <v>22.2</v>
@@ -3643,10 +3556,10 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2013</v>
       </c>
       <c r="C30" s="2">
         <v>17.8</v>
@@ -3750,10 +3663,10 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2011</v>
       </c>
       <c r="C31" s="2">
         <v>13.1</v>
@@ -3857,10 +3770,10 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2009</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>0</v>
@@ -3964,10 +3877,10 @@
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2006</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>0</v>
@@ -4071,10 +3984,10 @@
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2005</v>
       </c>
       <c r="C34" s="2">
         <v>11.8</v>
@@ -4178,10 +4091,10 @@
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1997</v>
       </c>
       <c r="C35" s="2">
         <v>12.9</v>
@@ -4283,10 +4196,10 @@
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1993</v>
       </c>
       <c r="C36" s="2">
         <v>7.5</v>
@@ -4388,10 +4301,10 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1986</v>
       </c>
       <c r="C37" s="2">
         <v>11.3</v>

</xml_diff>

<commit_message>
Changed the data AGAIN - LAYOUT IS BETTER FOR SQL DATABASE #ThisAgain
</commit_message>
<xml_diff>
--- a/EditedData.xlsx
+++ b/EditedData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="28">
   <si>
     <t/>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Indicator</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -495,11 +498,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="M19:V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -794,7 +797,9 @@
       <c r="AH3" s="2">
         <v>65.900000000000006</v>
       </c>
-      <c r="AI3" s="2"/>
+      <c r="AI3" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -899,7 +904,9 @@
       <c r="AH4" s="2">
         <v>59.9</v>
       </c>
-      <c r="AI4" s="2"/>
+      <c r="AI4" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1004,7 +1011,9 @@
       <c r="AH5" s="2">
         <v>55.1</v>
       </c>
-      <c r="AI5" s="2"/>
+      <c r="AI5" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1109,7 +1118,9 @@
       <c r="AH6" s="2">
         <v>47.8</v>
       </c>
-      <c r="AI6" s="2"/>
+      <c r="AI6" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1214,7 +1225,9 @@
       <c r="AH7" s="2">
         <v>38.4</v>
       </c>
-      <c r="AI7" s="2"/>
+      <c r="AI7" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1319,7 +1332,9 @@
       <c r="AH8" s="2">
         <v>30.8</v>
       </c>
-      <c r="AI8" s="2"/>
+      <c r="AI8" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1359,34 +1374,34 @@
         <v>44.9</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W9" s="2">
         <v>6.1</v>
@@ -1410,22 +1425,22 @@
         <v>33.200000000000003</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AI9" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -1638,7 +1653,9 @@
       <c r="AH11" s="2">
         <v>23</v>
       </c>
-      <c r="AI11" s="2"/>
+      <c r="AI11" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1743,7 +1760,9 @@
       <c r="AH12" s="2">
         <v>15.2</v>
       </c>
-      <c r="AI12" s="2"/>
+      <c r="AI12" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -2169,7 +2188,9 @@
       <c r="AH16" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="AI16" s="2"/>
+      <c r="AI16" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -2274,7 +2295,9 @@
       <c r="AH17" s="2">
         <v>17.7</v>
       </c>
-      <c r="AI17" s="2"/>
+      <c r="AI17" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2356,13 +2379,13 @@
         <v>53.5</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD18" s="2">
         <v>20</v>
@@ -2379,7 +2402,9 @@
       <c r="AH18" s="2">
         <v>14</v>
       </c>
-      <c r="AI18" s="2"/>
+      <c r="AI18" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -2419,34 +2444,34 @@
         <v>30.5</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W19" s="2">
         <v>22.3</v>
@@ -2461,31 +2486,31 @@
         <v>57.4</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AH19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AI19" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
@@ -2496,76 +2521,76 @@
         <v>2015</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AA20" s="2">
         <v>5.0999999999999996</v>
@@ -3019,7 +3044,9 @@
       <c r="AH24" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="AI24" s="2"/>
+      <c r="AI24" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -3124,7 +3151,9 @@
       <c r="AH25" s="2">
         <v>7.1</v>
       </c>
-      <c r="AI25" s="2"/>
+      <c r="AI25" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -3164,34 +3193,34 @@
         <v>19.7</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W26" s="2">
         <v>16.399999999999999</v>
@@ -3215,22 +3244,22 @@
         <v>23.3</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AF26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AG26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AH26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AI26" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -3527,13 +3556,13 @@
         <v>35.700000000000003</v>
       </c>
       <c r="AA29" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC29" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD29" s="2">
         <v>25.7</v>
@@ -3741,13 +3770,13 @@
         <v>40.299999999999997</v>
       </c>
       <c r="AA31" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AC31" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AD31" s="2">
         <v>20.399999999999999</v>
@@ -3776,76 +3805,76 @@
         <v>2009</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Z32" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AA32" s="2">
         <v>3.3</v>
@@ -3883,76 +3912,76 @@
         <v>2006</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Z33" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AA33" s="2">
         <v>4.2</v>
@@ -4192,7 +4221,9 @@
       <c r="AH35" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AI35" s="2"/>
+      <c r="AI35" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -4297,7 +4328,9 @@
       <c r="AH36" s="2">
         <v>4.7</v>
       </c>
-      <c r="AI36" s="2"/>
+      <c r="AI36" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -4337,34 +4370,34 @@
         <v>1.7</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="W37" s="2">
         <v>18</v>
@@ -4388,22 +4421,22 @@
         <v>41.5</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AE37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AF37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AG37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AH37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AI37" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>